<commit_message>
Projekta caurskatīšana un pielabošana, GATAVS PROJEKTS
</commit_message>
<xml_diff>
--- a/LVT_Eksamens_TP_V_1_0_2.xlsx
+++ b/LVT_Eksamens_TP_V_1_0_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="266">
   <si>
     <t>Identifikatoru atšifrējums:</t>
   </si>
@@ -825,6 +825,12 @@
   </si>
   <si>
     <t>Kods izies cauri algoritman un masīvā asked saglabāsies 10 nedublēti cipari</t>
+  </si>
+  <si>
+    <t>TZ</t>
+  </si>
+  <si>
+    <t>Testēšanas žurnāls</t>
   </si>
 </sst>
 </file>
@@ -976,7 +982,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1024,32 +1030,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1069,18 +1050,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1106,9 +1075,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1123,8 +1089,49 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1421,21 +1428,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1"/>
@@ -1444,20 +1451,20 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
@@ -1486,175 +1493,185 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>111</v>
+      <c r="A21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>179</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="4"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1683,8 +1700,8 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="55"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
@@ -1695,10 +1712,10 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="55"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
@@ -1733,10 +1750,10 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="30"/>
+      <c r="B9" s="55"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="6" t="s">
@@ -1747,10 +1764,10 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="30"/>
+      <c r="B11" s="55"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6" t="s">
@@ -1801,10 +1818,10 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="30"/>
+      <c r="B18" s="55"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="6" t="s">
@@ -1815,8 +1832,8 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="31"/>
-      <c r="B20" s="30"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="55"/>
     </row>
     <row r="21" spans="1:2" ht="37.5" customHeight="1">
       <c r="A21" s="8"/>
@@ -1851,7 +1868,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="7" width="25.7109375" customWidth="1"/>
@@ -1885,64 +1902,64 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" ht="60">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="33" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="46"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
     </row>
     <row r="5" spans="1:8" ht="60">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="33" t="s">
         <v>81</v>
       </c>
       <c r="E5" s="22" t="s">
@@ -1951,25 +1968,25 @@
       <c r="F5" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="29" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="46"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="40" t="s">
         <v>86</v>
       </c>
       <c r="B7" s="22" t="s">
@@ -1990,12 +2007,12 @@
       <c r="G7" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="33" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="40" t="s">
         <v>94</v>
       </c>
       <c r="B8" s="22" t="s">
@@ -2016,22 +2033,22 @@
       <c r="G8" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="33" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="46"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
     </row>
     <row r="10" spans="1:8" ht="60">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="40" t="s">
         <v>97</v>
       </c>
       <c r="B10" s="22" t="s">
@@ -2052,12 +2069,12 @@
       <c r="G10" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="29" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="40" t="s">
         <v>98</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -2078,25 +2095,25 @@
       <c r="G11" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="29" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="46"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
     </row>
     <row r="13" spans="1:8" ht="45">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="33" t="s">
         <v>101</v>
       </c>
       <c r="C13" s="22" t="s">
@@ -2114,15 +2131,15 @@
       <c r="G13" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="42" t="s">
+      <c r="H13" s="33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="33" t="s">
         <v>101</v>
       </c>
       <c r="C14" s="22" t="s">
@@ -2140,202 +2157,202 @@
       <c r="G14" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="H14" s="42" t="s">
+      <c r="H14" s="33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="46"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
     </row>
     <row r="16" spans="1:8" ht="75">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="33" t="s">
         <v>120</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="33" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="46"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
     </row>
     <row r="18" spans="1:8" ht="120">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="G18" s="42" t="s">
+      <c r="G18" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="H18" s="42" t="s">
+      <c r="H18" s="33" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="90">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="46"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
     </row>
     <row r="21" spans="1:8" ht="105">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="G21" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="H21" s="42" t="s">
+      <c r="H21" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="46"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
     </row>
     <row r="23" spans="1:8" ht="45">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="33" t="s">
         <v>138</v>
       </c>
       <c r="F23" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="42" t="s">
+      <c r="G23" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="H23" s="42" t="s">
+      <c r="H23" s="33" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="46"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="49"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="49"/>
+      <c r="H25" s="36"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="50"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -2345,27 +2362,27 @@
       <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="49"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="49"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="50"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
@@ -2375,562 +2392,562 @@
       <c r="H29" s="22"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="42"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="42"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="64"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
     </row>
     <row r="33" spans="1:8" ht="75">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="D33" s="42" t="s">
+      <c r="D33" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="33" t="s">
         <v>142</v>
       </c>
       <c r="F33" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="G33" s="42" t="s">
+      <c r="G33" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="H33" s="42" t="s">
+      <c r="H33" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="46"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
     </row>
     <row r="35" spans="1:8" ht="60">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="33" t="s">
         <v>145</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="D35" s="42" t="s">
+      <c r="D35" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="33" t="s">
         <v>147</v>
       </c>
       <c r="F35" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="G35" s="42" t="s">
+      <c r="G35" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="H35" s="42" t="s">
+      <c r="H35" s="33" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="45">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="33" t="s">
         <v>148</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="D36" s="42" t="s">
+      <c r="D36" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="33" t="s">
         <v>154</v>
       </c>
       <c r="F36" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="G36" s="42" t="s">
+      <c r="G36" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="H36" s="42" t="s">
+      <c r="H36" s="33" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="46"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
     </row>
     <row r="38" spans="1:8" ht="60">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="33" t="s">
         <v>161</v>
       </c>
       <c r="B38" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="D38" s="42" t="s">
+      <c r="D38" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="33" t="s">
         <v>155</v>
       </c>
       <c r="F38" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="G38" s="42" t="s">
+      <c r="G38" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="H38" s="42" t="s">
+      <c r="H38" s="33" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="45">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="33" t="s">
         <v>162</v>
       </c>
       <c r="B39" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="C39" s="42" t="s">
+      <c r="C39" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="D39" s="42" t="s">
+      <c r="D39" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="33" t="s">
         <v>154</v>
       </c>
       <c r="F39" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="G39" s="42" t="s">
+      <c r="G39" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="H39" s="42" t="s">
+      <c r="H39" s="33" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="46"/>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
+      <c r="A40" s="58"/>
+      <c r="B40" s="59"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
     </row>
     <row r="41" spans="1:8" ht="60">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="42" t="s">
+      <c r="C41" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="D41" s="42" t="s">
+      <c r="D41" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="33" t="s">
         <v>172</v>
       </c>
       <c r="F41" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="G41" s="42" t="s">
+      <c r="G41" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="H41" s="42" t="s">
+      <c r="H41" s="33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="45">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B42" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="C42" s="42" t="s">
+      <c r="C42" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="D42" s="42" t="s">
+      <c r="D42" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E42" s="33" t="s">
         <v>154</v>
       </c>
       <c r="F42" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="G42" s="42" t="s">
+      <c r="G42" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="H42" s="42" t="s">
+      <c r="H42" s="33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="46"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-    </row>
-    <row r="44" spans="1:8" ht="60">
-      <c r="A44" s="42" t="s">
+      <c r="A43" s="58"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="59"/>
+    </row>
+    <row r="44" spans="1:8" ht="45">
+      <c r="A44" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C44" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D44" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="E44" s="42" t="s">
+      <c r="E44" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="F44" s="42" t="s">
+      <c r="F44" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="G44" s="42" t="s">
+      <c r="G44" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="H44" s="42" t="s">
+      <c r="H44" s="33" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="46"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
     </row>
     <row r="46" spans="1:8" ht="30">
-      <c r="A46" s="42" t="s">
+      <c r="A46" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="42" t="s">
+      <c r="C46" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="D46" s="42" t="s">
+      <c r="D46" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="E46" s="42" t="s">
+      <c r="E46" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="F46" s="42" t="s">
+      <c r="F46" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="G46" s="42" t="s">
+      <c r="G46" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="H46" s="42" t="s">
+      <c r="H46" s="33" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="46"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="59"/>
+      <c r="H47" s="59"/>
     </row>
     <row r="48" spans="1:8" ht="105">
-      <c r="A48" s="52" t="s">
+      <c r="A48" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="42" t="s">
+      <c r="C48" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="D48" s="42" t="s">
+      <c r="D48" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="E48" s="42" t="s">
+      <c r="E48" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="F48" s="42" t="s">
+      <c r="F48" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="G48" s="42" t="s">
+      <c r="G48" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="H48" s="42" t="s">
+      <c r="H48" s="33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="46"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
+      <c r="H49" s="59"/>
     </row>
     <row r="50" spans="1:8" ht="90">
-      <c r="A50" s="52" t="s">
+      <c r="A50" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="B50" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="42" t="s">
+      <c r="C50" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="D50" s="42" t="s">
+      <c r="D50" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="E50" s="42" t="s">
+      <c r="E50" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="F50" s="42" t="s">
+      <c r="F50" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="G50" s="42" t="s">
+      <c r="G50" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="H50" s="42" t="s">
+      <c r="H50" s="33" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="46"/>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
+      <c r="A51" s="58"/>
+      <c r="B51" s="59"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="59"/>
+      <c r="H51" s="59"/>
     </row>
     <row r="52" spans="1:8" ht="105">
-      <c r="A52" s="52" t="s">
+      <c r="A52" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="42" t="s">
+      <c r="C52" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="D52" s="42" t="s">
+      <c r="D52" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="E52" s="42" t="s">
+      <c r="E52" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="F52" s="42" t="s">
+      <c r="F52" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="G52" s="42" t="s">
+      <c r="G52" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="H52" s="42" t="s">
+      <c r="H52" s="33" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="105">
-      <c r="A53" s="52" t="s">
+      <c r="A53" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B53" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C53" s="42" t="s">
+      <c r="C53" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="D53" s="42" t="s">
+      <c r="D53" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="E53" s="42" t="s">
+      <c r="E53" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="F53" s="42" t="s">
+      <c r="F53" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="G53" s="42" t="s">
+      <c r="G53" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="H53" s="42" t="s">
+      <c r="H53" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="46"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45"/>
+      <c r="A54" s="58"/>
+      <c r="B54" s="59"/>
+      <c r="C54" s="59"/>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
     </row>
     <row r="55" spans="1:8" ht="90">
-      <c r="A55" s="42" t="s">
+      <c r="A55" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C55" s="42" t="s">
+      <c r="C55" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="D55" s="42" t="s">
+      <c r="D55" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="E55" s="42" t="s">
+      <c r="E55" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="F55" s="42" t="s">
+      <c r="F55" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="G55" s="42" t="s">
+      <c r="G55" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="H55" s="42" t="s">
+      <c r="H55" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="46"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
+      <c r="A56" s="58"/>
+      <c r="B56" s="59"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="59"/>
+      <c r="F56" s="59"/>
+      <c r="G56" s="59"/>
+      <c r="H56" s="59"/>
     </row>
     <row r="57" spans="1:8" ht="75">
-      <c r="A57" s="42" t="s">
+      <c r="A57" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="D57" s="42" t="s">
+      <c r="D57" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="E57" s="42" t="s">
+      <c r="E57" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="F57" s="42" t="s">
+      <c r="F57" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="G57" s="42" t="s">
+      <c r="G57" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="H57" s="42" t="s">
+      <c r="H57" s="33" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="60">
-      <c r="A58" s="42" t="s">
+      <c r="A58" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="B58" s="42" t="s">
+      <c r="B58" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="42" t="s">
+      <c r="C58" s="33" t="s">
         <v>218</v>
       </c>
-      <c r="D58" s="42" t="s">
+      <c r="D58" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="E58" s="42" t="s">
+      <c r="E58" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="F58" s="42" t="s">
+      <c r="F58" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="G58" s="42" t="s">
+      <c r="G58" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="H58" s="42" t="s">
+      <c r="H58" s="33" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="46"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
+      <c r="A59" s="58"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59"/>
+      <c r="F59" s="59"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="59"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="20"/>
@@ -3017,9 +3034,9 @@
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
-      <c r="E68" s="56"/>
-      <c r="F68" s="56"/>
-      <c r="G68" s="56"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
       <c r="H68" s="7"/>
     </row>
     <row r="69" spans="1:8">
@@ -3027,9 +3044,9 @@
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
-      <c r="E69" s="56"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
       <c r="H69" s="7"/>
     </row>
     <row r="70" spans="1:8">
@@ -3037,21 +3054,21 @@
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="56"/>
-      <c r="F70" s="56"/>
-      <c r="G70" s="56"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
       <c r="H70" s="7"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="B71" s="33"/>
-      <c r="C71" s="33"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="63"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="57"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
+      <c r="E71" s="43"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="42"/>
       <c r="H71" s="7"/>
     </row>
     <row r="72" spans="1:8" ht="25.5">
@@ -3065,81 +3082,81 @@
         <v>53</v>
       </c>
       <c r="D72" s="1"/>
-      <c r="E72" s="59"/>
-      <c r="F72" s="59"/>
-      <c r="G72" s="59"/>
+      <c r="E72" s="45"/>
+      <c r="F72" s="45"/>
+      <c r="G72" s="45"/>
       <c r="H72" s="7"/>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="33" t="s">
         <v>140</v>
       </c>
       <c r="C73" s="15">
         <v>0.14814814814814814</v>
       </c>
       <c r="D73" s="1"/>
-      <c r="E73" s="56"/>
-      <c r="F73" s="56"/>
-      <c r="G73" s="60"/>
+      <c r="E73" s="42"/>
+      <c r="F73" s="42"/>
+      <c r="G73" s="46"/>
       <c r="H73" s="7"/>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="1"/>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="33" t="s">
         <v>145</v>
       </c>
       <c r="C74" s="15">
         <v>0.1111111111111111</v>
       </c>
       <c r="D74" s="1"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56"/>
-      <c r="G74" s="60"/>
+      <c r="E74" s="42"/>
+      <c r="F74" s="42"/>
+      <c r="G74" s="46"/>
       <c r="H74" s="7"/>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="24"/>
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="33" t="s">
         <v>148</v>
       </c>
       <c r="C75" s="15">
         <v>0.1111111111111111</v>
       </c>
       <c r="D75" s="24"/>
-      <c r="E75" s="56"/>
-      <c r="F75" s="56"/>
-      <c r="G75" s="60"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="46"/>
       <c r="H75" s="7"/>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="24"/>
-      <c r="B76" s="42" t="s">
+      <c r="B76" s="33" t="s">
         <v>161</v>
       </c>
       <c r="C76" s="15">
         <v>0.11111111111111099</v>
       </c>
       <c r="D76" s="24"/>
-      <c r="E76" s="56"/>
-      <c r="F76" s="56"/>
-      <c r="G76" s="60"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="46"/>
       <c r="H76" s="7"/>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="24"/>
-      <c r="B77" s="42" t="s">
+      <c r="B77" s="33" t="s">
         <v>261</v>
       </c>
       <c r="C77" s="15">
         <v>0.11111111111111099</v>
       </c>
       <c r="D77" s="24"/>
-      <c r="E77" s="56"/>
-      <c r="F77" s="56"/>
-      <c r="G77" s="60"/>
+      <c r="E77" s="42"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="46"/>
       <c r="H77" s="7"/>
     </row>
     <row r="78" spans="1:8">
@@ -3152,9 +3169,9 @@
         <v>0.59259259259259234</v>
       </c>
       <c r="D78" s="1"/>
-      <c r="E78" s="56"/>
-      <c r="F78" s="56"/>
-      <c r="G78" s="56"/>
+      <c r="E78" s="42"/>
+      <c r="F78" s="42"/>
+      <c r="G78" s="42"/>
       <c r="H78" s="7"/>
     </row>
     <row r="79" spans="1:8">
@@ -3162,9 +3179,9 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
-      <c r="E79" s="63"/>
-      <c r="F79" s="56"/>
-      <c r="G79" s="56"/>
+      <c r="E79" s="49"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="42"/>
       <c r="H79" s="7"/>
     </row>
     <row r="80" spans="1:8" ht="25.5">
@@ -3178,16 +3195,16 @@
         <v>53</v>
       </c>
       <c r="D80" s="1"/>
-      <c r="E80" s="59"/>
-      <c r="F80" s="59"/>
-      <c r="G80" s="59"/>
+      <c r="E80" s="45"/>
+      <c r="F80" s="45"/>
+      <c r="G80" s="45"/>
       <c r="H80" s="7"/>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="33" t="s">
         <v>174</v>
       </c>
       <c r="C81" s="16">
@@ -3195,9 +3212,9 @@
         <v>1</v>
       </c>
       <c r="D81" s="1"/>
-      <c r="E81" s="56"/>
-      <c r="F81" s="37"/>
-      <c r="G81" s="62"/>
+      <c r="E81" s="42"/>
+      <c r="F81" s="28"/>
+      <c r="G81" s="48"/>
       <c r="H81" s="7"/>
     </row>
     <row r="82" spans="1:8">
@@ -3210,9 +3227,9 @@
         <v>1</v>
       </c>
       <c r="D82" s="1"/>
-      <c r="E82" s="56"/>
-      <c r="F82" s="37"/>
-      <c r="G82" s="62"/>
+      <c r="E82" s="42"/>
+      <c r="F82" s="28"/>
+      <c r="G82" s="48"/>
       <c r="H82" s="7"/>
     </row>
     <row r="83" spans="1:8">
@@ -3220,9 +3237,9 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
-      <c r="E83" s="56"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="62"/>
+      <c r="E83" s="42"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="48"/>
       <c r="H83" s="7"/>
     </row>
     <row r="84" spans="1:8" ht="25.5">
@@ -3236,16 +3253,16 @@
         <v>53</v>
       </c>
       <c r="D84" s="1"/>
-      <c r="E84" s="56"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="62"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="28"/>
+      <c r="G84" s="48"/>
       <c r="H84" s="7"/>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="B85" s="42" t="s">
+      <c r="B85" s="33" t="s">
         <v>182</v>
       </c>
       <c r="C85" s="16">
@@ -3253,9 +3270,9 @@
         <v>1</v>
       </c>
       <c r="D85" s="1"/>
-      <c r="E85" s="56"/>
-      <c r="F85" s="58"/>
-      <c r="G85" s="61"/>
+      <c r="E85" s="42"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="47"/>
       <c r="H85" s="7"/>
     </row>
     <row r="86" spans="1:8">
@@ -3303,7 +3320,7 @@
       <c r="A89" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="B89" s="52" t="s">
+      <c r="B89" s="39" t="s">
         <v>176</v>
       </c>
       <c r="C89" s="16">
@@ -3371,7 +3388,7 @@
       <c r="A94" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="B94" s="42" t="s">
+      <c r="B94" s="33" t="s">
         <v>175</v>
       </c>
       <c r="C94" s="16">
@@ -3386,7 +3403,7 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" s="1"/>
-      <c r="B95" s="52" t="s">
+      <c r="B95" s="39" t="s">
         <v>177</v>
       </c>
       <c r="C95" s="16">
@@ -3401,7 +3418,7 @@
     </row>
     <row r="96" spans="1:8">
       <c r="A96" s="1"/>
-      <c r="B96" s="52" t="s">
+      <c r="B96" s="39" t="s">
         <v>180</v>
       </c>
       <c r="C96" s="16">
@@ -3416,7 +3433,7 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="1"/>
-      <c r="B97" s="52" t="s">
+      <c r="B97" s="39" t="s">
         <v>181</v>
       </c>
       <c r="C97" s="16">
@@ -3431,7 +3448,7 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98" s="1"/>
-      <c r="B98" s="42" t="s">
+      <c r="B98" s="33" t="s">
         <v>183</v>
       </c>
       <c r="C98" s="16">
@@ -3461,12 +3478,14 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A56:H56"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A54:H54"/>
     <mergeCell ref="A43:H43"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A20:H20"/>
@@ -3476,14 +3495,12 @@
     <mergeCell ref="A34:H34"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A47:H47"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="A51:H51"/>
-    <mergeCell ref="A54:H54"/>
-    <mergeCell ref="A56:H56"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3494,9 +3511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3543,477 +3560,477 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="30">
         <v>44724</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="46"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="30">
         <v>44724</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F5" s="54" t="s">
+      <c r="F5" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="38"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="46"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="30">
         <v>44724</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="31" t="s">
         <v>86</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="38"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="30">
         <v>44724</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="31" t="s">
         <v>94</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="30">
         <v>44724</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="31" t="s">
         <v>97</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="30">
         <v>44724</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="31" t="s">
         <v>98</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F11" s="54" t="s">
+      <c r="F11" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="43"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" ht="30">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="B13" s="39">
+      <c r="B13" s="30">
         <v>44724</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="44.25" customHeight="1">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B14" s="30">
         <v>44724</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="A15" s="43"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="39" customHeight="1">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="29" t="s">
         <v>230</v>
       </c>
-      <c r="B16" s="39">
+      <c r="B16" s="30">
         <v>44724</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
-      <c r="A17" s="43"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="36.75" customHeight="1">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="B18" s="39">
+      <c r="B18" s="30">
         <v>44724</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="41.25" customHeight="1">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="B19" s="39">
+      <c r="B19" s="30">
         <v>44724</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F19" s="54" t="s">
+      <c r="F19" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1">
-      <c r="A20" s="43"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="B21" s="39">
+      <c r="B21" s="30">
         <v>44724</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F21" s="54" t="s">
+      <c r="F21" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1">
-      <c r="A22" s="43"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
+      <c r="A22" s="64"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="39" customHeight="1">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="B23" s="39">
+      <c r="B23" s="30">
         <v>44724</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1">
-      <c r="A24" s="43"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="87.75" customHeight="1">
-      <c r="A25" s="47"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1">
-      <c r="A26" s="50"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -4026,33 +4043,33 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="45.75" customHeight="1">
-      <c r="A27" s="47"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="39" customHeight="1">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1">
-      <c r="A29" s="50"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
@@ -4065,579 +4082,579 @@
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1">
-      <c r="A30" s="38"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" ht="30" customHeight="1">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B32" s="51">
+      <c r="B32" s="38">
         <v>44724</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F32" s="54" t="s">
+      <c r="F32" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:11" ht="18" customHeight="1">
-      <c r="A33" s="46"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" ht="30" customHeight="1">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="B34" s="51">
+      <c r="B34" s="38">
         <v>44724</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="33" t="s">
         <v>145</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F34" s="54" t="s">
+      <c r="F34" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" ht="30" customHeight="1">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="B35" s="51">
+      <c r="B35" s="38">
         <v>44724</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="33" t="s">
         <v>148</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F35" s="54" t="s">
+      <c r="F35" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A36" s="46"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
       <c r="I36" s="24"/>
       <c r="J36" s="24"/>
       <c r="K36" s="24"/>
     </row>
     <row r="37" spans="1:11" ht="30" customHeight="1">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="33" t="s">
         <v>239</v>
       </c>
-      <c r="B37" s="51">
+      <c r="B37" s="38">
         <v>44724</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="33" t="s">
         <v>161</v>
       </c>
       <c r="D37" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E37" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F37" s="54" t="s">
+      <c r="F37" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11" ht="30" customHeight="1">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="B38" s="51">
+      <c r="B38" s="38">
         <v>44724</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="33" t="s">
         <v>162</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F38" s="54" t="s">
+      <c r="F38" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A39" s="46"/>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="59"/>
       <c r="I39" s="24"/>
       <c r="J39" s="24"/>
       <c r="K39" s="24"/>
     </row>
     <row r="40" spans="1:11" ht="30" customHeight="1">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="B40" s="51">
+      <c r="B40" s="38">
         <v>44724</v>
       </c>
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="33" t="s">
         <v>169</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F40" s="54" t="s">
+      <c r="F40" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
     <row r="41" spans="1:11" ht="30" customHeight="1">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="B41" s="51">
+      <c r="B41" s="38">
         <v>44724</v>
       </c>
-      <c r="C41" s="42" t="s">
+      <c r="C41" s="33" t="s">
         <v>169</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F41" s="54" t="s">
+      <c r="F41" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
     <row r="42" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A42" s="46"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
       <c r="I42" s="24"/>
       <c r="J42" s="24"/>
       <c r="K42" s="24"/>
     </row>
     <row r="43" spans="1:11" ht="30" customHeight="1">
-      <c r="A43" s="42" t="s">
+      <c r="A43" s="33" t="s">
         <v>243</v>
       </c>
-      <c r="B43" s="51">
+      <c r="B43" s="38">
         <v>44724</v>
       </c>
-      <c r="C43" s="42" t="s">
+      <c r="C43" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="D43" s="42" t="s">
+      <c r="D43" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F43" s="54" t="s">
+      <c r="F43" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
     <row r="44" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A44" s="46"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
+      <c r="A44" s="58"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
       <c r="I44" s="24"/>
       <c r="J44" s="24"/>
       <c r="K44" s="24"/>
     </row>
     <row r="45" spans="1:11" ht="30" customHeight="1">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="B45" s="51">
+      <c r="B45" s="38">
         <v>44724</v>
       </c>
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D45" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="42" t="s">
+      <c r="E45" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F45" s="54" t="s">
+      <c r="F45" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
     <row r="46" spans="1:11" ht="18" customHeight="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
     <row r="47" spans="1:11" ht="30" customHeight="1">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="B47" s="51">
+      <c r="B47" s="38">
         <v>44724</v>
       </c>
-      <c r="C47" s="52" t="s">
+      <c r="C47" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="D47" s="42" t="s">
+      <c r="D47" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="42" t="s">
+      <c r="E47" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F47" s="54" t="s">
+      <c r="F47" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A48" s="46"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
+      <c r="A48" s="58"/>
+      <c r="B48" s="59"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="59"/>
+      <c r="H48" s="59"/>
       <c r="I48" s="24"/>
       <c r="J48" s="24"/>
       <c r="K48" s="24"/>
     </row>
     <row r="49" spans="1:11" ht="30" customHeight="1">
-      <c r="A49" s="42" t="s">
+      <c r="A49" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="B49" s="51">
+      <c r="B49" s="38">
         <v>44724</v>
       </c>
-      <c r="C49" s="52" t="s">
+      <c r="C49" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="D49" s="42" t="s">
+      <c r="D49" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="E49" s="42" t="s">
+      <c r="E49" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F49" s="54" t="s">
+      <c r="F49" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
     <row r="50" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A50" s="46"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
+      <c r="A50" s="58"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
       <c r="I50" s="24"/>
       <c r="J50" s="24"/>
       <c r="K50" s="24"/>
     </row>
     <row r="51" spans="1:11" ht="30" customHeight="1">
-      <c r="A51" s="42" t="s">
+      <c r="A51" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="B51" s="51">
+      <c r="B51" s="38">
         <v>44724</v>
       </c>
-      <c r="C51" s="52" t="s">
+      <c r="C51" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="D51" s="42" t="s">
+      <c r="D51" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="42" t="s">
+      <c r="E51" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F51" s="54" t="s">
+      <c r="F51" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
     <row r="52" spans="1:11" ht="45" customHeight="1">
-      <c r="A52" s="52" t="s">
+      <c r="A52" s="39" t="s">
         <v>248</v>
       </c>
-      <c r="B52" s="51">
+      <c r="B52" s="38">
         <v>44724</v>
       </c>
-      <c r="C52" s="52" t="s">
+      <c r="C52" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="D52" s="42" t="s">
+      <c r="D52" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="E52" s="42" t="s">
+      <c r="E52" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F52" s="54" t="s">
+      <c r="F52" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
     <row r="53" spans="1:11" ht="18" customHeight="1">
-      <c r="A53" s="46"/>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="45"/>
-      <c r="G53" s="45"/>
-      <c r="H53" s="45"/>
+      <c r="A53" s="58"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="59"/>
+      <c r="H53" s="59"/>
       <c r="I53" s="24"/>
       <c r="J53" s="24"/>
       <c r="K53" s="24"/>
     </row>
     <row r="54" spans="1:11" ht="45" customHeight="1">
-      <c r="A54" s="52" t="s">
+      <c r="A54" s="39" t="s">
         <v>249</v>
       </c>
-      <c r="B54" s="51">
+      <c r="B54" s="38">
         <v>44724</v>
       </c>
-      <c r="C54" s="42" t="s">
+      <c r="C54" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="D54" s="42" t="s">
+      <c r="D54" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="E54" s="42" t="s">
+      <c r="E54" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F54" s="54" t="s">
+      <c r="F54" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A55" s="46"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
+      <c r="A55" s="58"/>
+      <c r="B55" s="59"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" ht="45" customHeight="1">
-      <c r="A56" s="52" t="s">
+      <c r="A56" s="39" t="s">
         <v>250</v>
       </c>
-      <c r="B56" s="51">
+      <c r="B56" s="38">
         <v>44724</v>
       </c>
-      <c r="C56" s="42" t="s">
+      <c r="C56" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="D56" s="42" t="s">
+      <c r="D56" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="42" t="s">
+      <c r="E56" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F56" s="54" t="s">
+      <c r="F56" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="1:11" ht="45" customHeight="1">
-      <c r="A57" s="52" t="s">
+      <c r="A57" s="39" t="s">
         <v>251</v>
       </c>
-      <c r="B57" s="51">
+      <c r="B57" s="38">
         <v>44724</v>
       </c>
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="D57" s="42" t="s">
+      <c r="D57" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="E57" s="42" t="s">
+      <c r="E57" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="F57" s="54" t="s">
+      <c r="F57" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="G57" s="42"/>
-      <c r="H57" s="42"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
     <row r="58" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A58" s="46"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
+      <c r="A58" s="58"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
+      <c r="F58" s="59"/>
+      <c r="G58" s="59"/>
+      <c r="H58" s="59"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
     <row r="59" spans="1:11" ht="45" customHeight="1">
       <c r="A59" s="11"/>
-      <c r="B59" s="35"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="23"/>
       <c r="D59" s="23"/>
       <c r="E59" s="23"/>
@@ -4650,7 +4667,7 @@
     </row>
     <row r="60" spans="1:11" ht="45" customHeight="1">
       <c r="A60" s="11"/>
-      <c r="B60" s="35"/>
+      <c r="B60" s="26"/>
       <c r="C60" s="23"/>
       <c r="D60" s="23"/>
       <c r="E60" s="23"/>
@@ -4663,7 +4680,7 @@
     </row>
     <row r="61" spans="1:11" ht="45" customHeight="1">
       <c r="A61" s="11"/>
-      <c r="B61" s="35"/>
+      <c r="B61" s="26"/>
       <c r="C61" s="23"/>
       <c r="D61" s="23"/>
       <c r="E61" s="23"/>
@@ -4676,20 +4693,20 @@
     </row>
     <row r="62" spans="1:11" ht="18" customHeight="1">
       <c r="A62" s="20"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="27"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
     <row r="63" spans="1:11" ht="45" customHeight="1">
       <c r="A63" s="11"/>
-      <c r="B63" s="35"/>
+      <c r="B63" s="26"/>
       <c r="C63" s="23"/>
       <c r="D63" s="23"/>
       <c r="E63" s="23"/>
@@ -4702,7 +4719,7 @@
     </row>
     <row r="64" spans="1:11" ht="45" customHeight="1">
       <c r="A64" s="11"/>
-      <c r="B64" s="35"/>
+      <c r="B64" s="26"/>
       <c r="C64" s="23"/>
       <c r="D64" s="23"/>
       <c r="E64" s="23"/>
@@ -4715,20 +4732,20 @@
     </row>
     <row r="65" spans="1:11" ht="19.5" customHeight="1">
       <c r="A65" s="20"/>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="36"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="27"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
     <row r="66" spans="1:11" ht="45" customHeight="1">
       <c r="A66" s="11"/>
-      <c r="B66" s="35"/>
+      <c r="B66" s="26"/>
       <c r="C66" s="23"/>
       <c r="D66" s="23"/>
       <c r="E66" s="23"/>
@@ -4741,7 +4758,7 @@
     </row>
     <row r="67" spans="1:11" ht="45" customHeight="1">
       <c r="A67" s="11"/>
-      <c r="B67" s="35"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="23"/>
       <c r="D67" s="23"/>
       <c r="E67" s="23"/>
@@ -4754,13 +4771,13 @@
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1">
       <c r="A68" s="20"/>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="36"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
@@ -4851,12 +4868,11 @@
     <row r="80" spans="1:11" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A58:H58"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A50:H50"/>
+    <mergeCell ref="A53:H53"/>
     <mergeCell ref="A46:H46"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A20:H20"/>
@@ -4868,11 +4884,12 @@
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A42:H42"/>
     <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="A58:H58"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A50:H50"/>
-    <mergeCell ref="A53:H53"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>